<commit_message>
Added MapReduce and comparison graphs
</commit_message>
<xml_diff>
--- a/415PasswordCrackerData.xlsx
+++ b/415PasswordCrackerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.stowman\Desktop\Password-Hacker-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyler.svendsen\Desktop\Password-Hacker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Password</t>
   </si>
@@ -222,6 +222,12 @@
   <si>
     <t>Brute Force Singlethread (Days)</t>
   </si>
+  <si>
+    <t>Multithread</t>
+  </si>
+  <si>
+    <t>MapReduce</t>
+  </si>
 </sst>
 </file>
 
@@ -276,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -285,6 +291,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1696,6 +1704,1103 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Multiple Passwords'!$B$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Map Reduce</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$A$30:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$B$30:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>171</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95B1-4419-97FA-1EE6E5DCFBB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="297857640"/>
+        <c:axId val="297859280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="297857640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Passwords</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297859280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="297859280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297857640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Between Mutlithread and MapReduce</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Multiple Passwords'!$B$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multithread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$A$44:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$B$44:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.47486</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7089999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.265000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.978999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.951000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.593999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110.577</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>193.61199999999999</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>294.10899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91B4-4F95-9DCA-F49023C803F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Multiple Passwords'!$C$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MapReduce</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$A$44:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Multiple Passwords'!$C$44:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>171</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-91B4-4F95-9DCA-F49023C803F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="297857312"/>
+        <c:axId val="297857968"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="297857312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Passwords</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297857968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="297857968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="297857312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -1813,6 +2918,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2969,6 +4154,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3409,6 +5626,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4719,11 +6996,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,7 +7057,7 @@
         <v>50</v>
       </c>
       <c r="B4" s="6">
-        <f t="shared" ref="B4:B14" si="0">$B$2*A4</f>
+        <f t="shared" ref="B4:B13" si="0">$B$2*A4</f>
         <v>2116.701</v>
       </c>
       <c r="C4" s="6">
@@ -5088,9 +7365,252 @@
         <v>3.6748281249999999</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>50</v>
+      </c>
+      <c r="B32" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>100</v>
+      </c>
+      <c r="B33" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>250</v>
+      </c>
+      <c r="B34" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>500</v>
+      </c>
+      <c r="B35" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>750</v>
+      </c>
+      <c r="B36" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1000</v>
+      </c>
+      <c r="B37" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2000</v>
+      </c>
+      <c r="B38" s="9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3000</v>
+      </c>
+      <c r="B39" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5000</v>
+      </c>
+      <c r="B40" s="9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>7500</v>
+      </c>
+      <c r="B41" s="9">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>1</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0.47486</v>
+      </c>
+      <c r="C44" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1.998</v>
+      </c>
+      <c r="C45" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>50</v>
+      </c>
+      <c r="B46" s="6">
+        <v>2.6760000000000002</v>
+      </c>
+      <c r="C46" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>100</v>
+      </c>
+      <c r="B47" s="6">
+        <v>4.7089999999999996</v>
+      </c>
+      <c r="C47" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>250</v>
+      </c>
+      <c r="B48" s="6">
+        <v>10.265000000000001</v>
+      </c>
+      <c r="C48" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>500</v>
+      </c>
+      <c r="B49" s="6">
+        <v>19.978999999999999</v>
+      </c>
+      <c r="C49" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>750</v>
+      </c>
+      <c r="B50" s="6">
+        <v>29.131</v>
+      </c>
+      <c r="C50" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1000</v>
+      </c>
+      <c r="B51" s="6">
+        <v>36.951000000000001</v>
+      </c>
+      <c r="C51" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2000</v>
+      </c>
+      <c r="B52" s="6">
+        <v>73.593999999999994</v>
+      </c>
+      <c r="C52" s="9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3000</v>
+      </c>
+      <c r="B53" s="6">
+        <v>110.577</v>
+      </c>
+      <c r="C53" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>5000</v>
+      </c>
+      <c r="B54">
+        <v>193.61199999999999</v>
+      </c>
+      <c r="C54" s="9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>7500</v>
+      </c>
+      <c r="B55">
+        <v>294.10899999999998</v>
+      </c>
+      <c r="C55" s="9">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5162,7 +7682,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B13" si="0">B6*B6</f>
+        <f t="shared" ref="B7:B11" si="0">B6*B6</f>
         <v>3211925.8518718025</v>
       </c>
     </row>

</xml_diff>